<commit_message>
📃 docs(All): Slightly optimized.
</commit_message>
<xml_diff>
--- a/OutData/sec_I_0.0_y/ModelManager_sec_I.xlsx
+++ b/OutData/sec_I_0.0_y/ModelManager_sec_I.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,34 +422,34 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>tag</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>group</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -481,7 +469,7 @@
       <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -501,7 +489,7 @@
       <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -521,7 +509,7 @@
       <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -541,7 +529,7 @@
       <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -557,7 +545,7 @@
       <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -577,7 +565,7 @@
       <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -601,7 +589,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="inlineStr">

</xml_diff>